<commit_message>
Mise à jour recodage domaines HAL
</commit_message>
<xml_diff>
--- a/HAL_in/Recodage domaines HAL-sections CNU.xlsx
+++ b/HAL_in/Recodage domaines HAL-sections CNU.xlsx
@@ -348,892 +348,892 @@
     <t xml:space="preserve">phys.nucl = Physique [physics]/Physique Nucléaire Théorique [nucl-th]</t>
   </si>
   <si>
+    <t xml:space="preserve">phys.grqc = Physique [physics]/Relativité Générale et Cosmologie Quantique [gr-qc]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-acc-ph = Physique [physics]/Physique [physics]/Physique des accélérateurs [physics.acc-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nlin.nlin-cd = Science non linéaire [physics]/Dynamique Chaotique [nlin.CD]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.astr.co = Physique [physics]/Astrophysique [astro-ph]/Cosmologie et astrophysique extra-galactique [astro-ph.CO]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Milieux dilués et optique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-optics = Physique [physics]/Physique [physics]/Optique [physics.optics]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-atm-ph = Physique [physics]/Physique [physics]/Agrégats Moléculaires et Atomiques [physics.atm-clus]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-plasm-ph = Physique [physics]/Physique [physics]/Physique des plasmas [physics.plasm-ph]</t>
+  </si>
+  <si>
     <t xml:space="preserve">phys.phys.phys-atom-ph = Physique [physics]/Physique [physics]/Physique Atomique [physics.atom-ph]</t>
   </si>
   <si>
+    <t xml:space="preserve">phys.phys.phys-chem-ph = Physique [physics]/Physique [physics]/Chimie-Physique [physics.chem-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chimie théorique, physique, analytique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.anal = Chimie/Chimie analytique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.theo = Chimie/Chimie théorique et/ou physique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chimie organique, inorganique, industrielle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.orga = Chimie/Chimie organique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.inor = Chimie/Chimie inorganique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.geni = Chimie/Génie chimique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chimie des matériaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.mate = Chimie/Matériaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.poly = Chimie/Polymères</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.cris = Chimie/Cristallographie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Astronomie, astrophysique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.astr = Physique [physics]/Astrophysique [astro-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.astr = Planète et Univers [physics]/Astrophysique [astro-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Structure et évolution de la Terre et des autres planètes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-geo-ph = Physique [physics]/Physique [physics]/Géophysique [physics.geo-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.ag = Planète et Univers [physics]/Sciences de la Terre/Géologie appliquée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.gc = Planète et Univers [physics]/Sciences de la Terre/Géochimie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.gm = Planète et Univers [physics]/Sciences de la Terre/Géomorphologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.hy = Planète et Univers [physics]/Sciences de la Terre/Hydrologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.mi = Planète et Univers [physics]/Sciences de la Terre/Minéralogie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.pe = Planète et Univers [physics]/Sciences de la Terre/Pétrographie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.pg = Planète et Univers [physics]/Sciences de la Terre/Paléontologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.pl = Planète et Univers [physics]/Sciences de la Terre/Planétologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.st = Planète et Univers [physics]/Sciences de la Terre/Stratigraphie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.te = Planète et Univers [physics]/Sciences de la Terre/Tectonique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.vo = Planète et Univers [physics]/Sciences de la Terre/Volcanologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terre solide : géodynamique des enveloppes supérieures, paléobiosphère</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Météorologie, océanographie physique et physique de l'environnement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.cl = Planète et Univers [physics]/Sciences de la Terre/Climatologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.gl = Planète et Univers [physics]/Sciences de la Terre/Glaciologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.gp = Planète et Univers [physics]/Sciences de la Terre/Géophysique [physics.geo-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.me = Planète et Univers [physics]/Sciences de la Terre/Météorologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.stu.oc = Planète et Univers [physics]/Sciences de la Terre/Océanographie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.ocean = Planète et Univers [physics]/Océan, Atmosphère</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdu.envi = Planète et Univers [physics]/Interfaces continentales, environnement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morphologie et morphogenèse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bdd.mor = Sciences du Vivant [q-bio]/Biologie du développement/Morphogenèse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.aha = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Anatomie, Histologie, Anatomopathologie [q-bio.TO]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biophysique et imagerie médicale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bbm.bp = Sciences du Vivant [q-bio]/Biochimie, Biologie Moléculaire/Biophysique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.ib.ima = Sciences du Vivant [q-bio]/Ingénierie biomédicale/Imagerie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.ib.mn = Sciences du Vivant [q-bio]/Ingénierie biomédicale/Médecine nucléaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biochimie, biologie cellulaire et moléculaire, physiologie et nutrition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bbm.bc = Sciences du Vivant [q-bio]/Biochimie, Biologie Moléculaire/Biochimie [q-bio.BM]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bc = Sciences du Vivant [q-bio]/Biologie cellulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.phy = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Physiologie [q-bio.TO]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.aen = Sciences du Vivant [q-bio]/Alimentation et Nutrition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.ida = Sciences du Vivant [q-bio]/Ingénierie des aliments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microbiologie, maladies transmissibles et hygiène</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mp = Sciences du Vivant [q-bio]/Microbiologie et Parasitologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.mi = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Maladies infectieuses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Santé publique, environnement et société</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.spee = Sciences du Vivant [q-bio]/Santé publique et épidémiologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sde.es = Sciences de l'environnement/Environnement et Société</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cancérologie, génétique, hématologie, immunologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.can = Sciences du Vivant [q-bio]/Cancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.hem = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Hématologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.imm = Sciences du Vivant [q-bio]/Immunologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.gen.gh = Sciences du Vivant [q-bio]/Génétique/Génétique humaine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anesthésiologie, réanimation, médecine d'urgence, pharmacologie et thérapeutique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.sp.pharma = Sciences du Vivant [q-bio]/Sciences pharmaceutiques/Pharmacologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep = Sciences du Vivant [q-bio]/Médecine humaine et pathologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathologie nerveuse et musculaire, pathologie mentale, handicap et rééducation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.psm = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Psychiatrie et santé mentale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.neu.nb = Sciences du Vivant [q-bio]/Neurosciences [q-bio.NC]/Neurobiologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathologie ostéo-articulaire, dermatologie et chirurgie plastique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.derm = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Dermatologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.rsoa = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Rhumatologie et système ostéo-articulaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathologie cardiorespiratoire et vasculaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.csc = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Cardiologie et système cardiovasculaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.psr = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Pneumologie et système respiratoire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maladies des appareils digestif et urinaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.heg = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Hépatologie et Gastroentérologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.un = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Urologie et Néphrologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Médecine interne, gériatrie, chirurgie générale et médecine générale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.chi = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Chirurgie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.geg = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Gériatrie et gérontologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Développement et pathologie de l'enfant, gynécologie-obstétrique, endocrinologie et reproduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.ped = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Pédiatrie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.geo = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Gynécologie et obstétrique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.em = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Endocrinologie et métabolisme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bdlr = Sciences du Vivant [q-bio]/Biologie de la reproduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pathologie de la tête et du cou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mhep.os = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Organes des sens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Développement, croissance et prévention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sciences biologiques, médecine et chirurgie buccales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bdd.eo = Sciences du Vivant [q-bio]/Biologie du développement/Embryologie et organogenèse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.mp.bac = Sciences du Vivant [q-bio]/Microbiologie et Parasitologie/Bactériologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sciences physiques et physiologiques endodontiques et prothétiques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.ib = Sciences du Vivant [q-bio]/Ingénierie biomédicale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-bio-ph = Physique [physics]/Physique [physics]/Biophysique [physics.bio-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mécanique, génie mécanique, génie civil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.meca = Physique [physics]/Mécanique [physics]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spi.meca = Sciences de l'ingénieur [physics]/Mécanique [physics.med-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spi.gciv = Sciences de l'ingénieur [physics]/Génie civil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Génie informatique, automatique et traitement du signal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spi.signal = Sciences de l'ingénieur [physics]/Traitement du signal et de l'image [eess.SP]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spi.auto = Sciences de l'ingénieur [physics]/Automatique / Robotique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Énergétique, génie des procédés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spi.nrj = Sciences de l'ingénieur [physics]/Energie électrique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spi.gproc = Sciences de l'ingénieur [physics]/Génie des procédés</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Génie Électrique, Électronique, optronique et systèmes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spi.opti = Sciences de l'ingénieur [physics]/Optique / photonique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spi.tron = Sciences de l'ingénieur [physics]/Electronique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biochimie et biologie moléculaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bbm = Sciences du Vivant [q-bio]/Biochimie, Biologie Moléculaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biologie cellulaire</t>
+  </si>
+  <si>
+    <t>Physiologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.ba = Sciences du Vivant [q-bio]/Biologie animale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bv = Sciences du Vivant [q-bio]/Biologie végétale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.tox.eco = Sciences du Vivant [q-bio]/Toxicologie/Ecotoxicologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biologie des populations et écologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sde.be = Sciences de l'environnement/Biodiversité et Ecologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bid = Sciences du Vivant [q-bio]/Biodiversité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.gen.gpo = Sciences du Vivant [q-bio]/Génétique/Génétique des populations [q-bio.PE]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-bi = Informatique [cs]/Bio-informatique [q-bio.QM]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biologie des organismes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.tox = Sciences du Vivant [q-bio]/Toxicologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bio = Sciences du Vivant [q-bio]/Biotechnologies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.sa = Sciences du Vivant [q-bio]/Sciences agricoles</t>
+  </si>
+  <si>
+    <t>Neurosciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.neu = Sciences du Vivant [q-bio]/Neurosciences [q-bio.NC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sciences de l'éducation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shs.edu = Sciences de l'Homme et Société/Education</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sciences de l'information et de la communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shs.info = Sciences de l'Homme et Société/Sciences de l'information et de la communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Épistémologie, histoire des sciences et des techniques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shs.hisphilso = Sciences de l'Homme et Société/Histoire, Philosophie et Sociologie des sciences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cultures et langues régionales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shs = Sciences de l'Homme et Société</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sciences et techniques des activités physiques et sportives</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Théologie catholique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shs.relig = Sciences de l'Homme et Société/Religions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Théologie protestante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sciences physico-chimiques et ingénierie appliquée à la santé (ex-39)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bibs = Sciences du Vivant [q-bio]/Bio-Informatique, Biologie Systémique [q-bio.QM]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.sp.pg = Sciences du Vivant [q-bio]/Sciences pharmaceutiques/Pharmacie galénique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.ib.bio = Sciences du Vivant [q-bio]/Ingénierie biomédicale/Biomatériaux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sciences du médicament et des autres produits de santé (ex-40)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.sp = Sciences du Vivant [q-bio]/Sciences pharmaceutiques</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sciences biologiques, fondamentales et cliniques (ex-41)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdv.bdd = Sciences du Vivant [q-bio]/Biologie du développement</t>
+  </si>
+  <si>
+    <t>Maïeutique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sciences de la rééducation et de la réadaptation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scco.psyc = Sciences cognitives/Psychologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sciences infirmières</t>
+  </si>
+  <si>
+    <t>label_s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim = Chimie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.cata = Chimie/Catalyse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.chem = Chimie/Chemo-informatique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.coor = Chimie/Chimie de coordination</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.othe = Chimie/Autre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.radio = Chimie/Radiochimie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chim.ther = Chimie/Chimie thérapeutique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.eiah = Informatique [cs]/Environnements Informatiques pour l'Apprentissage Humain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ai = Informatique [cs]/Intelligence artificielle [cs.AI]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ao = Informatique [cs]/Arithmétique des ordinateurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ar = Informatique [cs]/Architectures Matérielles [cs.AR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-au = Informatique [cs]/Automatique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-bt = Informatique [cs]/Biotechnologie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-cc = Informatique [cs]/Complexité [cs.CC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ce = Informatique [cs]/Ingénierie, finance et science [cs.CE]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-cg = Informatique [cs]/Géométrie algorithmique [cs.CG]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-cl = Informatique [cs]/Informatique et langage [cs.CL]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-cr = Informatique [cs]/Cryptographie et sécurité [cs.CR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-cv = Informatique [cs]/Vision par ordinateur et reconnaissance de formes [cs.CV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-cy = Informatique [cs]/Ordinateur et société [cs.CY]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-db = Informatique [cs]/Base de données [cs.DB]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-dc = Informatique [cs]/Calcul parallèle, distribué et partagé [cs.DC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-dl = Informatique [cs]/Bibliothèque électronique [cs.DL]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-dm = Informatique [cs]/Mathématique discrète [cs.DM]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ds = Informatique [cs]/Algorithme et structure de données [cs.DS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-es = Informatique [cs]/Systèmes embarqués</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-et = Informatique [cs]/Technologies Émergeantes [cs.ET]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-fl = Informatique [cs]/Théorie et langage formel [cs.FL]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-gl = Informatique [cs]/Littérature générale [cs.GL]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-gr = Informatique [cs]/Synthèse d'image et réalité virtuelle [cs.GR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-gt = Informatique [cs]/Informatique et théorie des jeux [cs.GT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-hc = Informatique [cs]/Interface homme-machine [cs.HC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ia = Informatique [cs]/Ingénierie assistée par ordinateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-im = Informatique [cs]/Imagerie médicale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ir = Informatique [cs]/Recherche d'information [cs.IR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-it = Informatique [cs]/Théorie de l'information [cs.IT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-iu = Informatique [cs]/Informatique ubiquitaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-lg = Informatique [cs]/Apprentissage [cs.LG]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-lo = Informatique [cs]/Logique en informatique [cs.LO]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ma = Informatique [cs]/Système multi-agents [cs.MA]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-mc = Informatique [cs]/Informatique mobile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-mm = Informatique [cs]/Multimédia [cs.MM]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-mo = Informatique [cs]/Modélisation et simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ms = Informatique [cs]/Logiciel mathématique [cs.MS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-na = Informatique [cs]/Analyse numérique [cs.NA]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ne = Informatique [cs]/Réseau de neurones [cs.NE]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ni = Informatique [cs]/Réseaux et télécommunications [cs.NI]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-oh = Informatique [cs]/Autre [cs.OH]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-os = Informatique [cs]/Système d'exploitation [cs.OS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-pf = Informatique [cs]/Performance et fiabilité [cs.PF]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-pl = Informatique [cs]/Langage de programmation [cs.PL]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-rb = Informatique [cs]/Robotique [cs.RO]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ro = Informatique [cs]/Recherche opérationnelle [cs.RO]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-sc = Informatique [cs]/Calcul formel [cs.SC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-sd = Informatique [cs]/Son [cs.SD]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-se = Informatique [cs]/Génie logiciel [cs.SE]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-si = Informatique [cs]/Réseaux sociaux et d'information [cs.SI]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-sy = Informatique [cs]/Systèmes et contrôle [cs.SY]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ti = Informatique [cs]/Traitement des images [eess.IV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-ts = Informatique [cs]/Traitement du signal et de l'image [eess.SP]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-tt = Informatique [cs]/Traitement du texte et du document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">info.info-wb = Informatique [cs]/Web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mathématiques appliquées</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-ac = Mathématiques [math]/Algèbre commutative [math.AC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-ag = Mathématiques [math]/Géométrie algébrique [math.AG]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-ap = Mathématiques [math]/Equations aux dérivées partielles [math.AP]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-at = Mathématiques [math]/Topologie algébrique [math.AT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-ca = Mathématiques [math]/Analyse classique [math.CA]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-co = Mathématiques [math]/Combinatoire [math.CO]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-ct = Mathématiques [math]/Catégories et ensembles [math.CT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-cv = Mathématiques [math]/Variables complexes [math.CV]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-dg = Mathématiques [math]/Géométrie différentielle [math.DG]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-ds = Mathématiques [math]/Systèmes dynamiques [math.DS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-fa = Mathématiques [math]/Analyse fonctionnelle [math.FA]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-gm = Mathématiques [math]/Mathématiques générales [math.GM]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-gn = Mathématiques [math]/Topologie générale [math.GN]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-gr = Mathématiques [math]/Théorie des groupes [math.GR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-gt = Mathématiques [math]/Topologie géométrique [math.GT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-ho = Mathématiques [math]/Histoire et perspectives sur les mathématiques [math.HO]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-it = Mathématiques [math]/Théorie de l'information et codage [math.IT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-kt = Mathématiques [math]/K-théorie et homologie [math.KT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-lo = Mathématiques [math]/Logique [math.LO]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-mg = Mathématiques [math]/Géométrie métrique [math.MG]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-mp = Mathématiques [math]/Physique mathématique [math-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-na = Mathématiques [math]/Analyse numérique [math.NA]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-nt = Mathématiques [math]/Théorie des nombres [math.NT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-oa = Mathématiques [math]/Algèbres d'opérateurs [math.OA]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-oc = Mathématiques [math]/Optimisation et contrôle [math.OC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-pr = Mathématiques [math]/Probabilités [math.PR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-qa = Mathématiques [math]/Algèbres quantiques [math.QA]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-ra = Mathématiques [math]/Anneaux et algèbres [math.RA]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-rt = Mathématiques [math]/Théorie des représentations [math.RT]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-sg = Mathématiques [math]/Géométrie symplectique [math.SG]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-sp = Mathématiques [math]/Théorie spectrale [math.SP]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">math.math-st = Mathématiques [math]/Statistiques [math.ST]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nlin = Science non linéaire [physics]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nlin.nlin-ao = Science non linéaire [physics]/Adaptation et Systèmes auto-organisés [nlin.AO]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nlin.nlin-cg = Science non linéaire [physics]/Automates cellulaires et gaz sur réseau [nlin.CG]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nlin.nlin-ps = Science non linéaire [physics]/Formation de Structures et Solitons [nlin.PS]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nlin.nlin-si = Science non linéaire [physics]/Systèmes Solubles et Intégrables [nlin.SI]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys = Physique [physics]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.astr.ep = Physique [physics]/Astrophysique [astro-ph]/Planétologie et astrophysique de la terre [astro-ph.EP]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.astr.ga = Physique [physics]/Astrophysique [astro-ph]/Astrophysique galactique [astro-ph.GA]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.astr.im = Physique [physics]/Astrophysique [astro-ph]/Instrumentation et méthodes pour l'astrophysique [astro-ph.IM]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.astr.sr = Physique [physics]/Astrophysique [astro-ph]/Astrophysique stellaire et solaire [astro-ph.SR]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.cond.cm-ds-nn = Physique [physics]/Matière Condensée [cond-mat]/Systèmes désordonnés et réseaux de neurones [cond-mat.dis-nn]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.cond.cm-gen = Physique [physics]/Matière Condensée [cond-mat]/Autre [cond-mat.other]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.cond.cm-ms = Physique [physics]/Matière Condensée [cond-mat]/Science des matériaux [cond-mat.mtrl-sci]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.cond.cm-msqhe = Physique [physics]/Matière Condensée [cond-mat]/Systèmes mésoscopiques et effet Hall quantique [cond-mat.mes-hall]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.cond.cm-s = Physique [physics]/Matière Condensée [cond-mat]/Supraconductivité [cond-mat.supr-con]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.cond.cm-sce = Physique [physics]/Matière Condensée [cond-mat]/Electrons fortement corrélés [cond-mat.str-el]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.cond.cm-scm = Physique [physics]/Matière Condensée [cond-mat]/Matière Molle [cond-mat.soft]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.cond.cm-sm = Physique [physics]/Matière Condensée [cond-mat]/Mécanique statistique [cond-mat.stat-mech]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.cond.gas = Physique [physics]/Matière Condensée [cond-mat]/Gaz Quantiques [cond-mat.quant-gas]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.hist = Physique [physics]/Articles anciens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.hlat = Physique [physics]/Physique des Hautes Energies - Réseau [hep-lat]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.hthe = Physique [physics]/Physique des Hautes Energies - Théorie [hep-th]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.meca.acou = Physique [physics]/Mécanique [physics]/Acoustique [physics.class-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.meca.biom = Physique [physics]/Mécanique [physics]/Biomécanique [physics.med-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.meca.geme = Physique [physics]/Mécanique [physics]/Génie mécanique [physics.class-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.meca.stru = Physique [physics]/Mécanique [physics]/Mécanique des structures [physics.class-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.meca.ther = Physique [physics]/Mécanique [physics]/Thermique [physics.class-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.meca.vibr = Physique [physics]/Mécanique [physics]/Vibrations [physics.class-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.mphy = Physique [physics]/Physique mathématique [math-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys = Physique [physics]/Physique [physics]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-ao-ph = Physique [physics]/Physique [physics]/Physique Atmosphérique et Océanique [physics.ao-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-class-ph = Physique [physics]/Physique [physics]/Physique Classique [physics.class-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-comp-ph = Physique [physics]/Physique [physics]/Physique Numérique [physics.comp-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-data-an = Physique [physics]/Physique [physics]/Analyse de données, Statistiques et Probabilités [physics.data-an]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-ed-ph = Physique [physics]/Physique [physics]/Enseignement de la physique [physics.ed-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-gen-ph = Physique [physics]/Physique [physics]/Physique Générale [physics.gen-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-hist-ph = Physique [physics]/Physique [physics]/Histoire de la Physique [physics.hist-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-ins-det = Physique [physics]/Physique [physics]/Instrumentations et Détecteurs [physics.ins-det]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-med-ph = Physique [physics]/Physique [physics]/Physique Médicale [physics.med-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-pop-ph = Physique [physics]/Physique [physics]/Physique : vulgarisation [physics.pop-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-soc-ph = Physique [physics]/Physique [physics]/Physique et Société [physics.soc-ph]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phys.phys.phys-space-ph = Physique [physics]/Physique [physics]/Physique de l'espace [physics.space-ph]</t>
+  </si>
+  <si>
     <t xml:space="preserve">phys.qphy = Physique [physics]/Physique Quantique [quant-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.grqc = Physique [physics]/Relativité Générale et Cosmologie Quantique [gr-qc]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Milieux dilués et optique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-optics = Physique [physics]/Physique [physics]/Optique [physics.optics]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-atm-ph = Physique [physics]/Physique [physics]/Agrégats Moléculaires et Atomiques [physics.atm-clus]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-plasm-ph = Physique [physics]/Physique [physics]/Physique des plasmas [physics.plasm-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-chem-ph = Physique [physics]/Physique [physics]/Chimie-Physique [physics.chem-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chimie théorique, physique, analytique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.anal = Chimie/Chimie analytique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.theo = Chimie/Chimie théorique et/ou physique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chimie organique, inorganique, industrielle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.orga = Chimie/Chimie organique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.inor = Chimie/Chimie inorganique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.geni = Chimie/Génie chimique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chimie des matériaux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.mate = Chimie/Matériaux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.poly = Chimie/Polymères</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.cris = Chimie/Cristallographie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Astronomie, astrophysique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.astr = Physique [physics]/Astrophysique [astro-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.astr = Planète et Univers [physics]/Astrophysique [astro-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Structure et évolution de la Terre et des autres planètes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-geo-ph = Physique [physics]/Physique [physics]/Géophysique [physics.geo-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.ag = Planète et Univers [physics]/Sciences de la Terre/Géologie appliquée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.gc = Planète et Univers [physics]/Sciences de la Terre/Géochimie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.gm = Planète et Univers [physics]/Sciences de la Terre/Géomorphologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.hy = Planète et Univers [physics]/Sciences de la Terre/Hydrologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.mi = Planète et Univers [physics]/Sciences de la Terre/Minéralogie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.pe = Planète et Univers [physics]/Sciences de la Terre/Pétrographie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.pg = Planète et Univers [physics]/Sciences de la Terre/Paléontologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.pl = Planète et Univers [physics]/Sciences de la Terre/Planétologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.st = Planète et Univers [physics]/Sciences de la Terre/Stratigraphie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.te = Planète et Univers [physics]/Sciences de la Terre/Tectonique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.vo = Planète et Univers [physics]/Sciences de la Terre/Volcanologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Terre solide : géodynamique des enveloppes supérieures, paléobiosphère</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Météorologie, océanographie physique et physique de l'environnement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.cl = Planète et Univers [physics]/Sciences de la Terre/Climatologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.gl = Planète et Univers [physics]/Sciences de la Terre/Glaciologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.gp = Planète et Univers [physics]/Sciences de la Terre/Géophysique [physics.geo-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.me = Planète et Univers [physics]/Sciences de la Terre/Météorologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.stu.oc = Planète et Univers [physics]/Sciences de la Terre/Océanographie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.ocean = Planète et Univers [physics]/Océan, Atmosphère</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdu.envi = Planète et Univers [physics]/Interfaces continentales, environnement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Morphologie et morphogenèse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bdd.mor = Sciences du Vivant [q-bio]/Biologie du développement/Morphogenèse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.aha = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Anatomie, Histologie, Anatomopathologie [q-bio.TO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biophysique et imagerie médicale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bbm.bp = Sciences du Vivant [q-bio]/Biochimie, Biologie Moléculaire/Biophysique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.ib.ima = Sciences du Vivant [q-bio]/Ingénierie biomédicale/Imagerie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.ib.mn = Sciences du Vivant [q-bio]/Ingénierie biomédicale/Médecine nucléaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biochimie, biologie cellulaire et moléculaire, physiologie et nutrition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bbm.bc = Sciences du Vivant [q-bio]/Biochimie, Biologie Moléculaire/Biochimie [q-bio.BM]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bc = Sciences du Vivant [q-bio]/Biologie cellulaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.phy = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Physiologie [q-bio.TO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.aen = Sciences du Vivant [q-bio]/Alimentation et Nutrition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.ida = Sciences du Vivant [q-bio]/Ingénierie des aliments</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microbiologie, maladies transmissibles et hygiène</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mp = Sciences du Vivant [q-bio]/Microbiologie et Parasitologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.mi = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Maladies infectieuses</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Santé publique, environnement et société</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.spee = Sciences du Vivant [q-bio]/Santé publique et épidémiologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sde.es = Sciences de l'environnement/Environnement et Société</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cancérologie, génétique, hématologie, immunologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.can = Sciences du Vivant [q-bio]/Cancer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.hem = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Hématologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.imm = Sciences du Vivant [q-bio]/Immunologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.gen.gh = Sciences du Vivant [q-bio]/Génétique/Génétique humaine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anesthésiologie, réanimation, médecine d'urgence, pharmacologie et thérapeutique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.sp.pharma = Sciences du Vivant [q-bio]/Sciences pharmaceutiques/Pharmacologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep = Sciences du Vivant [q-bio]/Médecine humaine et pathologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathologie nerveuse et musculaire, pathologie mentale, handicap et rééducation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.psm = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Psychiatrie et santé mentale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.neu.nb = Sciences du Vivant [q-bio]/Neurosciences [q-bio.NC]/Neurobiologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathologie ostéo-articulaire, dermatologie et chirurgie plastique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.derm = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Dermatologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.rsoa = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Rhumatologie et système ostéo-articulaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathologie cardiorespiratoire et vasculaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.csc = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Cardiologie et système cardiovasculaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.psr = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Pneumologie et système respiratoire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maladies des appareils digestif et urinaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.heg = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Hépatologie et Gastroentérologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.un = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Urologie et Néphrologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Médecine interne, gériatrie, chirurgie générale et médecine générale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.chi = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Chirurgie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.geg = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Gériatrie et gérontologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Développement et pathologie de l'enfant, gynécologie-obstétrique, endocrinologie et reproduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.ped = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Pédiatrie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.geo = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Gynécologie et obstétrique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.em = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Endocrinologie et métabolisme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bdlr = Sciences du Vivant [q-bio]/Biologie de la reproduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pathologie de la tête et du cou</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mhep.os = Sciences du Vivant [q-bio]/Médecine humaine et pathologie/Organes des sens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Développement, croissance et prévention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sciences biologiques, médecine et chirurgie buccales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bdd.eo = Sciences du Vivant [q-bio]/Biologie du développement/Embryologie et organogenèse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.mp.bac = Sciences du Vivant [q-bio]/Microbiologie et Parasitologie/Bactériologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sciences physiques et physiologiques endodontiques et prothétiques</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.ib = Sciences du Vivant [q-bio]/Ingénierie biomédicale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-bio-ph = Physique [physics]/Physique [physics]/Biophysique [physics.bio-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mécanique, génie mécanique, génie civil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.meca = Physique [physics]/Mécanique [physics]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spi.meca = Sciences de l'ingénieur [physics]/Mécanique [physics.med-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spi.gciv = Sciences de l'ingénieur [physics]/Génie civil</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Génie informatique, automatique et traitement du signal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spi.signal = Sciences de l'ingénieur [physics]/Traitement du signal et de l'image [eess.SP]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spi.auto = Sciences de l'ingénieur [physics]/Automatique / Robotique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Énergétique, génie des procédés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spi.nrj = Sciences de l'ingénieur [physics]/Energie électrique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spi.gproc = Sciences de l'ingénieur [physics]/Génie des procédés</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Génie Électrique, Électronique, optronique et systèmes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spi.opti = Sciences de l'ingénieur [physics]/Optique / photonique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spi.tron = Sciences de l'ingénieur [physics]/Electronique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biochimie et biologie moléculaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bbm = Sciences du Vivant [q-bio]/Biochimie, Biologie Moléculaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biologie cellulaire</t>
-  </si>
-  <si>
-    <t>Physiologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.ba = Sciences du Vivant [q-bio]/Biologie animale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bv = Sciences du Vivant [q-bio]/Biologie végétale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.tox.eco = Sciences du Vivant [q-bio]/Toxicologie/Ecotoxicologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biologie des populations et écologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sde.be = Sciences de l'environnement/Biodiversité et Ecologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bid = Sciences du Vivant [q-bio]/Biodiversité</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.gen.gpo = Sciences du Vivant [q-bio]/Génétique/Génétique des populations [q-bio.PE]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-bi = Informatique [cs]/Bio-informatique [q-bio.QM]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Biologie des organismes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.tox = Sciences du Vivant [q-bio]/Toxicologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bio = Sciences du Vivant [q-bio]/Biotechnologies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.sa = Sciences du Vivant [q-bio]/Sciences agricoles</t>
-  </si>
-  <si>
-    <t>Neurosciences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.neu = Sciences du Vivant [q-bio]/Neurosciences [q-bio.NC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sciences de l'éducation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shs.edu = Sciences de l'Homme et Société/Education</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sciences de l'information et de la communication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shs.info = Sciences de l'Homme et Société/Sciences de l'information et de la communication</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Épistémologie, histoire des sciences et des techniques</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shs.hisphilso = Sciences de l'Homme et Société/Histoire, Philosophie et Sociologie des sciences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cultures et langues régionales</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shs = Sciences de l'Homme et Société</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sciences et techniques des activités physiques et sportives</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Théologie catholique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shs.relig = Sciences de l'Homme et Société/Religions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Théologie protestante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sciences physico-chimiques et ingénierie appliquée à la santé (ex-39)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bibs = Sciences du Vivant [q-bio]/Bio-Informatique, Biologie Systémique [q-bio.QM]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.sp.pg = Sciences du Vivant [q-bio]/Sciences pharmaceutiques/Pharmacie galénique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.ib.bio = Sciences du Vivant [q-bio]/Ingénierie biomédicale/Biomatériaux</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sciences du médicament et des autres produits de santé (ex-40)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.sp = Sciences du Vivant [q-bio]/Sciences pharmaceutiques</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sciences biologiques, fondamentales et cliniques (ex-41)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sdv.bdd = Sciences du Vivant [q-bio]/Biologie du développement</t>
-  </si>
-  <si>
-    <t>Maïeutique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sciences de la rééducation et de la réadaptation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scco.psyc = Sciences cognitives/Psychologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sciences infirmières</t>
-  </si>
-  <si>
-    <t>label_s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim = Chimie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.cata = Chimie/Catalyse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.chem = Chimie/Chemo-informatique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.coor = Chimie/Chimie de coordination</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.othe = Chimie/Autre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.radio = Chimie/Radiochimie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chim.ther = Chimie/Chimie thérapeutique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.eiah = Informatique [cs]/Environnements Informatiques pour l'Apprentissage Humain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ai = Informatique [cs]/Intelligence artificielle [cs.AI]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ao = Informatique [cs]/Arithmétique des ordinateurs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ar = Informatique [cs]/Architectures Matérielles [cs.AR]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-au = Informatique [cs]/Automatique</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-bt = Informatique [cs]/Biotechnologie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-cc = Informatique [cs]/Complexité [cs.CC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ce = Informatique [cs]/Ingénierie, finance et science [cs.CE]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-cg = Informatique [cs]/Géométrie algorithmique [cs.CG]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-cl = Informatique [cs]/Informatique et langage [cs.CL]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-cr = Informatique [cs]/Cryptographie et sécurité [cs.CR]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-cv = Informatique [cs]/Vision par ordinateur et reconnaissance de formes [cs.CV]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-cy = Informatique [cs]/Ordinateur et société [cs.CY]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-db = Informatique [cs]/Base de données [cs.DB]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-dc = Informatique [cs]/Calcul parallèle, distribué et partagé [cs.DC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-dl = Informatique [cs]/Bibliothèque électronique [cs.DL]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-dm = Informatique [cs]/Mathématique discrète [cs.DM]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ds = Informatique [cs]/Algorithme et structure de données [cs.DS]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-es = Informatique [cs]/Systèmes embarqués</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-et = Informatique [cs]/Technologies Émergeantes [cs.ET]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-fl = Informatique [cs]/Théorie et langage formel [cs.FL]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-gl = Informatique [cs]/Littérature générale [cs.GL]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-gr = Informatique [cs]/Synthèse d'image et réalité virtuelle [cs.GR]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-gt = Informatique [cs]/Informatique et théorie des jeux [cs.GT]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-hc = Informatique [cs]/Interface homme-machine [cs.HC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ia = Informatique [cs]/Ingénierie assistée par ordinateur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-im = Informatique [cs]/Imagerie médicale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ir = Informatique [cs]/Recherche d'information [cs.IR]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-it = Informatique [cs]/Théorie de l'information [cs.IT]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-iu = Informatique [cs]/Informatique ubiquitaire</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-lg = Informatique [cs]/Apprentissage [cs.LG]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-lo = Informatique [cs]/Logique en informatique [cs.LO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ma = Informatique [cs]/Système multi-agents [cs.MA]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-mc = Informatique [cs]/Informatique mobile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-mm = Informatique [cs]/Multimédia [cs.MM]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-mo = Informatique [cs]/Modélisation et simulation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ms = Informatique [cs]/Logiciel mathématique [cs.MS]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-na = Informatique [cs]/Analyse numérique [cs.NA]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ne = Informatique [cs]/Réseau de neurones [cs.NE]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ni = Informatique [cs]/Réseaux et télécommunications [cs.NI]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-oh = Informatique [cs]/Autre [cs.OH]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-os = Informatique [cs]/Système d'exploitation [cs.OS]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-pf = Informatique [cs]/Performance et fiabilité [cs.PF]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-pl = Informatique [cs]/Langage de programmation [cs.PL]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-rb = Informatique [cs]/Robotique [cs.RO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ro = Informatique [cs]/Recherche opérationnelle [cs.RO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-sc = Informatique [cs]/Calcul formel [cs.SC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-sd = Informatique [cs]/Son [cs.SD]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-se = Informatique [cs]/Génie logiciel [cs.SE]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-si = Informatique [cs]/Réseaux sociaux et d'information [cs.SI]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-sy = Informatique [cs]/Systèmes et contrôle [cs.SY]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ti = Informatique [cs]/Traitement des images [eess.IV]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-ts = Informatique [cs]/Traitement du signal et de l'image [eess.SP]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-tt = Informatique [cs]/Traitement du texte et du document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">info.info-wb = Informatique [cs]/Web</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mathématiques appliquées</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-ac = Mathématiques [math]/Algèbre commutative [math.AC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-ag = Mathématiques [math]/Géométrie algébrique [math.AG]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-ap = Mathématiques [math]/Equations aux dérivées partielles [math.AP]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-at = Mathématiques [math]/Topologie algébrique [math.AT]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-ca = Mathématiques [math]/Analyse classique [math.CA]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-co = Mathématiques [math]/Combinatoire [math.CO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-ct = Mathématiques [math]/Catégories et ensembles [math.CT]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-cv = Mathématiques [math]/Variables complexes [math.CV]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-dg = Mathématiques [math]/Géométrie différentielle [math.DG]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-ds = Mathématiques [math]/Systèmes dynamiques [math.DS]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-fa = Mathématiques [math]/Analyse fonctionnelle [math.FA]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-gm = Mathématiques [math]/Mathématiques générales [math.GM]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-gn = Mathématiques [math]/Topologie générale [math.GN]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-gr = Mathématiques [math]/Théorie des groupes [math.GR]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-gt = Mathématiques [math]/Topologie géométrique [math.GT]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-ho = Mathématiques [math]/Histoire et perspectives sur les mathématiques [math.HO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-it = Mathématiques [math]/Théorie de l'information et codage [math.IT]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-kt = Mathématiques [math]/K-théorie et homologie [math.KT]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-lo = Mathématiques [math]/Logique [math.LO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-mg = Mathématiques [math]/Géométrie métrique [math.MG]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-mp = Mathématiques [math]/Physique mathématique [math-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-na = Mathématiques [math]/Analyse numérique [math.NA]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-nt = Mathématiques [math]/Théorie des nombres [math.NT]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-oa = Mathématiques [math]/Algèbres d'opérateurs [math.OA]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-oc = Mathématiques [math]/Optimisation et contrôle [math.OC]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-pr = Mathématiques [math]/Probabilités [math.PR]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-qa = Mathématiques [math]/Algèbres quantiques [math.QA]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-ra = Mathématiques [math]/Anneaux et algèbres [math.RA]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-rt = Mathématiques [math]/Théorie des représentations [math.RT]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-sg = Mathématiques [math]/Géométrie symplectique [math.SG]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-sp = Mathématiques [math]/Théorie spectrale [math.SP]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">math.math-st = Mathématiques [math]/Statistiques [math.ST]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nlin = Science non linéaire [physics]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nlin.nlin-ao = Science non linéaire [physics]/Adaptation et Systèmes auto-organisés [nlin.AO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nlin.nlin-cd = Science non linéaire [physics]/Dynamique Chaotique [nlin.CD]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nlin.nlin-cg = Science non linéaire [physics]/Automates cellulaires et gaz sur réseau [nlin.CG]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nlin.nlin-ps = Science non linéaire [physics]/Formation de Structures et Solitons [nlin.PS]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nlin.nlin-si = Science non linéaire [physics]/Systèmes Solubles et Intégrables [nlin.SI]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys = Physique [physics]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.astr.co = Physique [physics]/Astrophysique [astro-ph]/Cosmologie et astrophysique extra-galactique [astro-ph.CO]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.astr.ep = Physique [physics]/Astrophysique [astro-ph]/Planétologie et astrophysique de la terre [astro-ph.EP]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.astr.ga = Physique [physics]/Astrophysique [astro-ph]/Astrophysique galactique [astro-ph.GA]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.astr.im = Physique [physics]/Astrophysique [astro-ph]/Instrumentation et méthodes pour l'astrophysique [astro-ph.IM]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.astr.sr = Physique [physics]/Astrophysique [astro-ph]/Astrophysique stellaire et solaire [astro-ph.SR]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.cond.cm-ds-nn = Physique [physics]/Matière Condensée [cond-mat]/Systèmes désordonnés et réseaux de neurones [cond-mat.dis-nn]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.cond.cm-gen = Physique [physics]/Matière Condensée [cond-mat]/Autre [cond-mat.other]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.cond.cm-ms = Physique [physics]/Matière Condensée [cond-mat]/Science des matériaux [cond-mat.mtrl-sci]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.cond.cm-msqhe = Physique [physics]/Matière Condensée [cond-mat]/Systèmes mésoscopiques et effet Hall quantique [cond-mat.mes-hall]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.cond.cm-s = Physique [physics]/Matière Condensée [cond-mat]/Supraconductivité [cond-mat.supr-con]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.cond.cm-sce = Physique [physics]/Matière Condensée [cond-mat]/Electrons fortement corrélés [cond-mat.str-el]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.cond.cm-scm = Physique [physics]/Matière Condensée [cond-mat]/Matière Molle [cond-mat.soft]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.cond.cm-sm = Physique [physics]/Matière Condensée [cond-mat]/Mécanique statistique [cond-mat.stat-mech]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.cond.gas = Physique [physics]/Matière Condensée [cond-mat]/Gaz Quantiques [cond-mat.quant-gas]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.hist = Physique [physics]/Articles anciens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.hlat = Physique [physics]/Physique des Hautes Energies - Réseau [hep-lat]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.hthe = Physique [physics]/Physique des Hautes Energies - Théorie [hep-th]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.meca.acou = Physique [physics]/Mécanique [physics]/Acoustique [physics.class-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.meca.biom = Physique [physics]/Mécanique [physics]/Biomécanique [physics.med-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.meca.geme = Physique [physics]/Mécanique [physics]/Génie mécanique [physics.class-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.meca.stru = Physique [physics]/Mécanique [physics]/Mécanique des structures [physics.class-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.meca.ther = Physique [physics]/Mécanique [physics]/Thermique [physics.class-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.meca.vibr = Physique [physics]/Mécanique [physics]/Vibrations [physics.class-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.mphy = Physique [physics]/Physique mathématique [math-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys = Physique [physics]/Physique [physics]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-acc-ph = Physique [physics]/Physique [physics]/Physique des accélérateurs [physics.acc-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-ao-ph = Physique [physics]/Physique [physics]/Physique Atmosphérique et Océanique [physics.ao-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-class-ph = Physique [physics]/Physique [physics]/Physique Classique [physics.class-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-comp-ph = Physique [physics]/Physique [physics]/Physique Numérique [physics.comp-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-data-an = Physique [physics]/Physique [physics]/Analyse de données, Statistiques et Probabilités [physics.data-an]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-ed-ph = Physique [physics]/Physique [physics]/Enseignement de la physique [physics.ed-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-gen-ph = Physique [physics]/Physique [physics]/Physique Générale [physics.gen-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-hist-ph = Physique [physics]/Physique [physics]/Histoire de la Physique [physics.hist-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-ins-det = Physique [physics]/Physique [physics]/Instrumentations et Détecteurs [physics.ins-det]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-med-ph = Physique [physics]/Physique [physics]/Physique Médicale [physics.med-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-pop-ph = Physique [physics]/Physique [physics]/Physique : vulgarisation [physics.pop-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-soc-ph = Physique [physics]/Physique [physics]/Physique et Société [physics.soc-ph]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">phys.phys.phys-space-ph = Physique [physics]/Physique [physics]/Physique de l'espace [physics.space-ph]</t>
   </si>
   <si>
     <t xml:space="preserve">qfin.cp = Économie et finance quantitative [q-fin]/Finance quantitative [q-fin.CP]</t>
@@ -1579,7 +1579,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.000000"/>
       <color theme="1"/>
@@ -1594,10 +1594,6 @@
       <sz val="10.000000"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10.000000"/>
-      <name val="Times New Roman"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1633,7 +1629,7 @@
     <xf fontId="1" fillId="0" borderId="0" numFmtId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
       <protection hidden="0" locked="1"/>
     </xf>
@@ -1657,10 +1653,6 @@
     </xf>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="3" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left"/>
       <protection hidden="0" locked="1"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyProtection="0">
@@ -1687,7 +1679,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <person displayName="Anonyme" id="{949C2AFD-BFE5-B49F-68EA-CB5A9B9E33F0}" userId="uid-1741861003916" providerId="Teamlab"/>
+  <person displayName="Anonyme" id="{83874AC4-2326-C648-AACA-1C5B0DF4100B}" userId="uid-1741861003916" providerId="Teamlab"/>
 </personList>
 </file>
 
@@ -2101,19 +2093,19 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="B45" dT="2025-04-08T08:27:39.09Z" personId="{949C2AFD-BFE5-B49F-68EA-CB5A9B9E33F0}" id="{0E32E31C-D20E-0909-042A-4CE5D95820AB}" done="0">
+  <threadedComment ref="B45" dT="2025-04-08T08:27:39.09Z" personId="{83874AC4-2326-C648-AACA-1C5B0DF4100B}" id="{0E32E31C-D20E-0909-042A-4CE5D95820AB}" done="0">
     <text xml:space="preserve">Impossible de trouver des domaines sur l'anesthésie.
 </text>
   </threadedComment>
-  <threadedComment ref="B46" dT="2025-04-08T09:22:48.30Z" personId="{949C2AFD-BFE5-B49F-68EA-CB5A9B9E33F0}" id="{6450D489-4E74-1B36-1129-53ACB78C6CD7}" done="0">
+  <threadedComment ref="B46" dT="2025-04-08T09:22:48.30Z" personId="{83874AC4-2326-C648-AACA-1C5B0DF4100B}" id="{6450D489-4E74-1B36-1129-53ACB78C6CD7}" done="0">
     <text xml:space="preserve">Pas trop trouvé de trucs pour la rééducation. Voir aussi 91.
 </text>
   </threadedComment>
-  <threadedComment ref="E57" dT="2025-04-08T08:53:46.45Z" personId="{949C2AFD-BFE5-B49F-68EA-CB5A9B9E33F0}" id="{997FE3B7-5D16-AF7A-E7DC-C87111CBFE06}" done="0">
+  <threadedComment ref="E57" dT="2025-04-08T08:53:46.45Z" personId="{83874AC4-2326-C648-AACA-1C5B0DF4100B}" id="{997FE3B7-5D16-AF7A-E7DC-C87111CBFE06}" done="0">
     <text xml:space="preserve">Peut-être trop large ?
 </text>
   </threadedComment>
-  <threadedComment ref="C58" dT="2025-04-08T08:56:18.54Z" personId="{949C2AFD-BFE5-B49F-68EA-CB5A9B9E33F0}" id="{0A5696C4-8582-0282-88FA-BF44A4C7ACF8}" done="0">
+  <threadedComment ref="C58" dT="2025-04-08T08:56:18.54Z" personId="{83874AC4-2326-C648-AACA-1C5B0DF4100B}" id="{0A5696C4-8582-0282-88FA-BF44A4C7ACF8}" done="0">
     <text xml:space="preserve">Un peu restreint mais je trouve rien d'autre sur l'énergie. Peut-être Thermique ?
 </text>
   </threadedComment>
@@ -2123,8 +2115,8 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A71" zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView topLeftCell="A23" zoomScale="100" workbookViewId="0">
+      <selection activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
@@ -2564,6 +2556,9 @@
       <c r="J30" s="4" t="s">
         <v>79</v>
       </c>
+      <c r="K30" s="4" t="s">
+        <v>80</v>
+      </c>
       <c r="L30" s="4"/>
     </row>
     <row r="31" s="4" customFormat="1" ht="12.5">
@@ -2571,55 +2566,60 @@
         <v>30</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I31" s="7"/>
+        <v>86</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
     </row>
     <row r="32" ht="12.5">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I32"/>
+      <c r="J32"/>
     </row>
     <row r="33" ht="12.5">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E33" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" ht="12.5">
@@ -2627,16 +2627,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C34" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D34" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" ht="12.5">
@@ -2644,13 +2644,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D35" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" s="4" customFormat="1" ht="25">
@@ -2658,43 +2658,43 @@
         <v>35</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H36" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" s="4" customFormat="1" ht="25">
@@ -2702,41 +2702,41 @@
         <v>36</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H37" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="J37" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" s="4" customFormat="1" ht="25">
@@ -2744,31 +2744,31 @@
         <v>37</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="G38" s="4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H38" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="I38" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J38" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" ht="12.5">
@@ -2776,13 +2776,13 @@
         <v>42</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C39" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D39" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" ht="12.5">
@@ -2790,16 +2790,16 @@
         <v>43</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C40" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D40" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E40" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="41" ht="25">
@@ -2807,22 +2807,22 @@
         <v>44</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="C41" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D41" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E41" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F41" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="G41" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" ht="25">
@@ -2830,13 +2830,13 @@
         <v>45</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C42" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D42" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" ht="12.5">
@@ -2844,13 +2844,13 @@
         <v>46</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C43" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D43" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" ht="25">
@@ -2858,19 +2858,19 @@
         <v>47</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C44" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D44" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="E44" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F44" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" ht="25">
@@ -2878,13 +2878,13 @@
         <v>48</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C45" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D45" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="46" ht="37.5">
@@ -2892,13 +2892,13 @@
         <v>49</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C46" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D46" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" ht="25">
@@ -2906,13 +2906,13 @@
         <v>50</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C47" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D47" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="48" ht="12.5">
@@ -2920,13 +2920,13 @@
         <v>51</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C48" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D48" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="49" ht="12.5">
@@ -2934,13 +2934,13 @@
         <v>52</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D49" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" ht="25">
@@ -2948,13 +2948,13 @@
         <v>53</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C50" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D50" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" ht="37.5">
@@ -2962,19 +2962,19 @@
         <v>54</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="C51" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D51" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E51" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="F51" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G51"/>
     </row>
@@ -2983,13 +2983,13 @@
         <v>55</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C52" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D52" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="53" ht="12.5">
@@ -2997,13 +2997,13 @@
         <v>56</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C53" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D53" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" ht="25">
@@ -3011,28 +3011,28 @@
         <v>57</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C54" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D54" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E54" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F54" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G54" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H54" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="I54" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="55" ht="25">
@@ -3040,16 +3040,16 @@
         <v>58</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="C55" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D55" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E55" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" ht="12.5">
@@ -3057,16 +3057,16 @@
         <v>60</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D56" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E56" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="57" ht="25">
@@ -3074,13 +3074,13 @@
         <v>61</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="C57" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D57" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E57" t="s">
         <v>63</v>
@@ -3091,13 +3091,13 @@
         <v>62</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C58" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D58" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="59" ht="25">
@@ -3105,16 +3105,16 @@
         <v>63</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C59" t="s">
         <v>187</v>
       </c>
-      <c r="C59" t="s">
-        <v>185</v>
-      </c>
       <c r="D59" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="E59" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="60" ht="12.5">
@@ -3122,10 +3122,10 @@
         <v>64</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C60" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="61" ht="12.5">
@@ -3133,10 +3133,10 @@
         <v>65</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C61" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="62" s="4" customFormat="1" ht="12.5">
@@ -3144,22 +3144,22 @@
         <v>66</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" ht="12.5">
@@ -3167,22 +3167,22 @@
         <v>67</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C63" t="s">
+        <v>200</v>
+      </c>
+      <c r="D63" t="s">
+        <v>201</v>
+      </c>
+      <c r="E63" t="s">
+        <v>202</v>
+      </c>
+      <c r="F63" t="s">
         <v>198</v>
       </c>
-      <c r="D63" t="s">
-        <v>199</v>
-      </c>
-      <c r="E63" t="s">
-        <v>200</v>
-      </c>
-      <c r="F63" t="s">
-        <v>196</v>
-      </c>
       <c r="G63" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="64" s="0" customFormat="1" ht="12.5">
@@ -3190,19 +3190,19 @@
         <v>68</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C64" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D64" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E64" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F64" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="65" ht="12.5">
@@ -3210,10 +3210,10 @@
         <v>69</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C65" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="F65"/>
     </row>
@@ -3222,10 +3222,10 @@
         <v>70</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C66" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="67" ht="25">
@@ -3233,10 +3233,10 @@
         <v>71</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C67" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" ht="25">
@@ -3244,10 +3244,10 @@
         <v>72</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C68" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="69" ht="12.5">
@@ -3255,26 +3255,26 @@
         <v>73</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>215</v>
+        <v>216</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>217</v>
       </c>
       <c r="D69"/>
-      <c r="E69" s="8"/>
+      <c r="E69" s="7"/>
     </row>
     <row r="70" ht="25">
       <c r="A70" s="2">
         <v>74</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C70" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D70" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E70" t="s">
         <v>25</v>
@@ -3285,10 +3285,10 @@
         <v>76</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C71" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72" ht="12.5">
@@ -3296,10 +3296,10 @@
         <v>77</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C72" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="73" ht="25">
@@ -3307,19 +3307,19 @@
         <v>80</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C73" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D73" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E73" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="F73" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="74" ht="25">
@@ -3327,19 +3327,19 @@
         <v>81</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C74" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D74" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E74" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F74" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="75" ht="25">
@@ -3347,28 +3347,28 @@
         <v>82</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="C75" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D75" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E75" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="F75" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="G75" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H75" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="I75" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="76" ht="25">
@@ -3376,74 +3376,74 @@
         <v>85</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="D76" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="E76" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="F76" s="8" t="s">
+      <c r="C76" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D76" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
-      <c r="I76" s="8"/>
+      <c r="E76" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="F76" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+      <c r="I76" s="7"/>
     </row>
     <row r="77" ht="25">
       <c r="A77" s="2">
         <v>86</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>224</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="D77" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="E77" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>203</v>
-      </c>
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
-      <c r="I77" s="8"/>
+        <v>226</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="F77" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+      <c r="I77" s="7"/>
     </row>
     <row r="78" ht="25">
       <c r="A78" s="2">
         <v>87</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="D78" s="8" t="s">
-        <v>191</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G78" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="H78" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="I78" s="8" t="s">
-        <v>143</v>
+        <v>228</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="F78" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G78" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H78" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="79" ht="12.5">
@@ -3451,10 +3451,10 @@
         <v>90</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C79" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="80" ht="25">
@@ -3462,19 +3462,19 @@
         <v>91</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C80" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="C80" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D80" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E80" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F80" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81" ht="12.5">
@@ -3482,10 +3482,10 @@
         <v>92</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C81" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -3515,82 +3515,82 @@
   <sheetData>
     <row r="1" ht="12.800000000000001">
       <c r="A1" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" ht="12.800000000000001">
       <c r="A2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" ht="12.800000000000001">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" ht="12.800000000000001">
       <c r="A4" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="5" ht="12.800000000000001">
       <c r="A5" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" ht="12.800000000000001">
       <c r="A6" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" ht="12.800000000000001">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" ht="12.800000000000001">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" ht="12.800000000000001">
       <c r="A9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" ht="12.800000000000001">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" ht="12.800000000000001">
       <c r="A11" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" ht="12.800000000000001">
       <c r="A12" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" ht="12.800000000000001">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" ht="12.800000000000001">
       <c r="A14" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" ht="12.800000000000001">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" ht="12.800000000000001">
       <c r="A16" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
     </row>
     <row r="17" ht="12.800000000000001">
@@ -3600,282 +3600,282 @@
     </row>
     <row r="18" ht="12.800000000000001">
       <c r="A18" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="19" ht="12.800000000000001">
       <c r="A19" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" ht="12.800000000000001">
       <c r="A20" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" ht="12.800000000000001">
       <c r="A21" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" ht="12.800000000000001">
       <c r="A22" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="23" ht="12.800000000000001">
       <c r="A23" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="24" ht="12.800000000000001">
       <c r="A24" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" ht="12.800000000000001">
       <c r="A25" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" ht="12.800000000000001">
       <c r="A26" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" ht="12.800000000000001">
       <c r="A27" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" ht="12.800000000000001">
       <c r="A28" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" ht="12.800000000000001">
       <c r="A29" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="30" ht="12.800000000000001">
       <c r="A30" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" ht="12.800000000000001">
       <c r="A31" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" ht="12.800000000000001">
       <c r="A32" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" ht="12.800000000000001">
       <c r="A33" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" ht="12.800000000000001">
       <c r="A34" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row r="35" ht="12.800000000000001">
       <c r="A35" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="36" ht="12.800000000000001">
       <c r="A36" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" ht="12.800000000000001">
       <c r="A37" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row r="38" ht="12.800000000000001">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" ht="12.800000000000001">
       <c r="A39" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" ht="12.800000000000001">
       <c r="A40" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" ht="12.800000000000001">
       <c r="A41" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" ht="12.800000000000001">
       <c r="A42" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" ht="12.800000000000001">
       <c r="A43" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" ht="12.800000000000001">
       <c r="A44" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
     </row>
     <row r="45" ht="12.800000000000001">
       <c r="A45" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
     </row>
     <row r="46" ht="12.800000000000001">
       <c r="A46" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="47" ht="12.800000000000001">
       <c r="A47" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="48" ht="12.800000000000001">
       <c r="A48" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" ht="12.800000000000001">
       <c r="A49" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
     </row>
     <row r="50" ht="12.800000000000001">
       <c r="A50" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
     </row>
     <row r="51" ht="12.800000000000001">
       <c r="A51" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" ht="12.800000000000001">
       <c r="A52" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
     </row>
     <row r="53" ht="12.800000000000001">
       <c r="A53" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
     </row>
     <row r="54" ht="12.800000000000001">
       <c r="A54" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="55" ht="12.800000000000001">
       <c r="A55" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="56" ht="12.800000000000001">
       <c r="A56" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
     </row>
     <row r="57" ht="12.800000000000001">
       <c r="A57" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
     </row>
     <row r="58" ht="12.800000000000001">
       <c r="A58" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
     </row>
     <row r="59" ht="12.800000000000001">
       <c r="A59" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="60" ht="12.800000000000001">
       <c r="A60" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
     </row>
     <row r="61" ht="12.800000000000001">
       <c r="A61" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
     </row>
     <row r="62" ht="12.800000000000001">
       <c r="A62" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
     </row>
     <row r="63" ht="12.800000000000001">
       <c r="A63" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
     </row>
     <row r="64" ht="12.800000000000001">
       <c r="A64" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="65" ht="12.800000000000001">
       <c r="A65" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
     </row>
     <row r="66" ht="12.800000000000001">
       <c r="A66" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
     </row>
     <row r="67" ht="12.800000000000001">
       <c r="A67" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
     </row>
     <row r="68" ht="12.800000000000001">
       <c r="A68" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
     </row>
     <row r="69" ht="12.800000000000001">
       <c r="A69" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
     </row>
     <row r="70" ht="12.800000000000001">
       <c r="A70" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="71" ht="12.800000000000001">
       <c r="A71" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
     </row>
     <row r="72" ht="12.800000000000001">
       <c r="A72" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
     </row>
     <row r="73" ht="12.800000000000001">
       <c r="A73" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
     </row>
     <row r="74" ht="12.800000000000001">
@@ -3892,212 +3892,212 @@
         <v>26</v>
       </c>
       <c r="E74" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
     </row>
     <row r="75" ht="12.800000000000001">
       <c r="A75" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="76" ht="12.800000000000001">
       <c r="A76" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
     </row>
     <row r="77" ht="12.800000000000001">
       <c r="A77" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
     </row>
     <row r="78" ht="12.800000000000001">
       <c r="A78" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
     </row>
     <row r="79" ht="12.800000000000001">
       <c r="A79" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
     </row>
     <row r="80" ht="12.800000000000001">
       <c r="A80" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="81" ht="12.800000000000001">
       <c r="A81" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
     </row>
     <row r="82" ht="12.800000000000001">
       <c r="A82" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="83" ht="12.800000000000001">
       <c r="A83" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
     </row>
     <row r="84" ht="12.800000000000001">
       <c r="A84" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
     </row>
     <row r="85" ht="12.800000000000001">
       <c r="A85" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
     </row>
     <row r="86" ht="12.800000000000001">
       <c r="A86" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
     </row>
     <row r="87" ht="12.800000000000001">
       <c r="A87" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
     </row>
     <row r="88" ht="12.800000000000001">
       <c r="A88" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="89" ht="12.800000000000001">
       <c r="A89" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="90" ht="12.800000000000001">
       <c r="A90" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
     </row>
     <row r="91" ht="12.800000000000001">
       <c r="A91" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
     </row>
     <row r="92" ht="12.800000000000001">
       <c r="A92" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="93" ht="12.800000000000001">
       <c r="A93" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
     </row>
     <row r="94" ht="12.800000000000001">
       <c r="A94" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
     </row>
     <row r="95" ht="12.800000000000001">
       <c r="A95" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
     </row>
     <row r="96" ht="12.800000000000001">
       <c r="A96" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="97" ht="12.800000000000001">
       <c r="A97" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
     </row>
     <row r="98" ht="12.800000000000001">
       <c r="A98" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
     </row>
     <row r="99" ht="12.800000000000001">
       <c r="A99" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="100" ht="12.800000000000001">
       <c r="A100" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
     </row>
     <row r="101" ht="12.800000000000001">
       <c r="A101" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
     </row>
     <row r="102" ht="12.800000000000001">
       <c r="A102" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
     </row>
     <row r="103" ht="12.800000000000001">
       <c r="A103" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="104" ht="12.800000000000001">
       <c r="A104" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
     </row>
     <row r="105" ht="12.800000000000001">
       <c r="A105" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="106" ht="12.800000000000001">
       <c r="A106" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="107" ht="12.800000000000001">
       <c r="A107" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="108" ht="12.800000000000001">
       <c r="A108" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="109" ht="12.800000000000001">
       <c r="A109" t="s">
-        <v>330</v>
+        <v>79</v>
       </c>
     </row>
     <row r="110" ht="12.800000000000001">
       <c r="A110" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="111" ht="12.800000000000001">
       <c r="A111" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="112" ht="12.800000000000001">
       <c r="A112" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="113" ht="12.800000000000001">
       <c r="A113" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="114" ht="12.800000000000001">
       <c r="A114" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="115" ht="12.800000000000001">
       <c r="A115" t="s">
-        <v>335</v>
+        <v>80</v>
       </c>
     </row>
     <row r="116" ht="12.800000000000001">
@@ -4177,7 +4177,7 @@
     </row>
     <row r="131" ht="12.800000000000001">
       <c r="A131" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="132" ht="12.800000000000001">
@@ -4207,7 +4207,7 @@
     </row>
     <row r="137" ht="12.800000000000001">
       <c r="A137" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="138" ht="12.800000000000001">
@@ -4282,52 +4282,52 @@
     </row>
     <row r="152" ht="12.800000000000001">
       <c r="A152" t="s">
-        <v>360</v>
+        <v>78</v>
       </c>
     </row>
     <row r="153" ht="12.800000000000001">
       <c r="A153" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="154" ht="12.800000000000001">
       <c r="A154" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="155" ht="12.800000000000001">
       <c r="A155" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="156" ht="12.800000000000001">
       <c r="A156" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="157" ht="12.800000000000001">
       <c r="A157" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="158" ht="12.800000000000001">
       <c r="A158" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="159" ht="12.800000000000001">
       <c r="A159" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="160" ht="12.800000000000001">
       <c r="A160" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="161" ht="12.800000000000001">
       <c r="A161" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="162" ht="12.800000000000001">
@@ -4337,57 +4337,57 @@
     </row>
     <row r="163" ht="12.800000000000001">
       <c r="A163" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="164" ht="12.800000000000001">
       <c r="A164" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="165" ht="12.800000000000001">
       <c r="A165" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="166" ht="12.800000000000001">
       <c r="A166" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="167" ht="12.800000000000001">
       <c r="A167" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="168" ht="12.800000000000001">
       <c r="A168" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="169" ht="12.800000000000001">
       <c r="A169" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="170" ht="12.800000000000001">
       <c r="A170" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="171" ht="12.800000000000001">
       <c r="A171" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="172" ht="12.800000000000001">
       <c r="A172" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="173" ht="12.800000000000001">
       <c r="A173" t="s">
-        <v>78</v>
+        <v>372</v>
       </c>
     </row>
     <row r="174" ht="12.800000000000001">
@@ -4452,7 +4452,7 @@
     </row>
     <row r="186" ht="12.800000000000001">
       <c r="A186" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="187" ht="12.800000000000001">
@@ -4462,12 +4462,12 @@
     </row>
     <row r="188" ht="12.800000000000001">
       <c r="A188" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
     </row>
     <row r="189" ht="12.800000000000001">
       <c r="A189" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="190" ht="12.800000000000001">
@@ -4487,7 +4487,7 @@
     </row>
     <row r="193" ht="12.800000000000001">
       <c r="A193" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row r="194" ht="12.800000000000001">
@@ -4522,12 +4522,12 @@
     </row>
     <row r="200" ht="12.800000000000001">
       <c r="A200" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="201" ht="12.800000000000001">
       <c r="A201" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="202" ht="12.800000000000001">
@@ -4542,82 +4542,82 @@
     </row>
     <row r="204" ht="12.800000000000001">
       <c r="A204" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="205" ht="12.800000000000001">
       <c r="A205" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="206" ht="12.800000000000001">
       <c r="A206" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="207" ht="12.800000000000001">
       <c r="A207" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="208" ht="12.800000000000001">
       <c r="A208" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="209" ht="12.800000000000001">
       <c r="A209" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="210" ht="12.800000000000001">
       <c r="A210" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="211" ht="12.800000000000001">
       <c r="A211" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="212" ht="12.800000000000001">
       <c r="A212" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="213" ht="12.800000000000001">
       <c r="A213" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="214" ht="12.800000000000001">
       <c r="A214" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="215" ht="12.800000000000001">
       <c r="A215" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="216" ht="12.800000000000001">
       <c r="A216" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="217" ht="12.800000000000001">
       <c r="A217" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="218" ht="12.800000000000001">
       <c r="A218" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="219" ht="12.800000000000001">
       <c r="A219" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="220" ht="12.800000000000001">
@@ -4627,12 +4627,12 @@
     </row>
     <row r="221" ht="12.800000000000001">
       <c r="A221" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="222" ht="12.800000000000001">
       <c r="A222" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="223" ht="12.800000000000001">
@@ -4652,12 +4652,12 @@
     </row>
     <row r="226" ht="12.800000000000001">
       <c r="A226" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="227" ht="12.800000000000001">
       <c r="A227" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="228" ht="12.800000000000001">
@@ -4667,7 +4667,7 @@
     </row>
     <row r="229" ht="12.800000000000001">
       <c r="A229" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="230" ht="12.800000000000001">
@@ -4687,7 +4687,7 @@
     </row>
     <row r="233" ht="12.800000000000001">
       <c r="A233" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="234" ht="12.800000000000001">
@@ -4702,12 +4702,12 @@
     </row>
     <row r="236" ht="12.800000000000001">
       <c r="A236" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="237" ht="12.800000000000001">
       <c r="A237" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="238" ht="12.800000000000001">
@@ -4717,12 +4717,12 @@
     </row>
     <row r="239" ht="12.800000000000001">
       <c r="A239" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="240" ht="12.800000000000001">
       <c r="A240" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="241" ht="12.800000000000001">
@@ -4737,12 +4737,12 @@
     </row>
     <row r="243" ht="12.800000000000001">
       <c r="A243" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
     </row>
     <row r="244" ht="12.800000000000001">
       <c r="A244" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="245" ht="12.800000000000001">
@@ -4757,12 +4757,12 @@
     </row>
     <row r="247" ht="12.800000000000001">
       <c r="A247" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="248" ht="12.800000000000001">
       <c r="A248" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
     </row>
     <row r="249" ht="12.800000000000001">
@@ -4782,7 +4782,7 @@
     </row>
     <row r="252" ht="12.800000000000001">
       <c r="A252" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="253" ht="12.800000000000001">
@@ -4827,7 +4827,7 @@
     </row>
     <row r="261" ht="12.800000000000001">
       <c r="A261" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="262" ht="12.800000000000001">
@@ -4837,37 +4837,37 @@
     </row>
     <row r="263" ht="12.800000000000001">
       <c r="A263" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="264" ht="12.800000000000001">
       <c r="A264" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="265" ht="12.800000000000001">
       <c r="A265" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
     </row>
     <row r="266" ht="12.800000000000001">
       <c r="A266" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="267" ht="12.800000000000001">
       <c r="A267" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="268" ht="12.800000000000001">
       <c r="A268" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row r="269" ht="12.800000000000001">
       <c r="A269" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="270" ht="12.800000000000001">
@@ -4897,52 +4897,52 @@
     </row>
     <row r="275" ht="12.800000000000001">
       <c r="A275" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="276" ht="12.800000000000001">
       <c r="A276" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="277" ht="12.800000000000001">
       <c r="A277" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="278" ht="12.800000000000001">
       <c r="A278" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="279" ht="12.800000000000001">
       <c r="A279" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="280" ht="12.800000000000001">
       <c r="A280" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="281" ht="12.800000000000001">
       <c r="A281" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="282" ht="12.800000000000001">
       <c r="A282" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="283" ht="12.800000000000001">
       <c r="A283" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="284" ht="12.800000000000001">
       <c r="A284" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="285" ht="12.800000000000001">
@@ -4952,52 +4952,52 @@
     </row>
     <row r="286" ht="12.800000000000001">
       <c r="A286" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="287" ht="12.800000000000001">
       <c r="A287" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="288" ht="12.800000000000001">
       <c r="A288" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="289" ht="12.800000000000001">
       <c r="A289" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="290" ht="12.800000000000001">
       <c r="A290" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="291" ht="12.800000000000001">
       <c r="A291" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="292" ht="12.800000000000001">
       <c r="A292" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
     </row>
     <row r="293" ht="12.800000000000001">
       <c r="A293" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="294" ht="12.800000000000001">
       <c r="A294" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="295" ht="12.800000000000001">
       <c r="A295" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="296" ht="12.800000000000001">
@@ -5022,12 +5022,12 @@
     </row>
     <row r="300" ht="12.800000000000001">
       <c r="A300" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
     </row>
     <row r="301" ht="12.800000000000001">
       <c r="A301" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="302" ht="12.800000000000001">
@@ -5047,7 +5047,7 @@
     </row>
     <row r="305" ht="12.800000000000001">
       <c r="A305" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="306" ht="12.800000000000001">
@@ -5097,7 +5097,7 @@
     </row>
     <row r="315" ht="12.800000000000001">
       <c r="A315" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="316" ht="12.800000000000001">
@@ -5107,27 +5107,27 @@
     </row>
     <row r="317" ht="12.800000000000001">
       <c r="A317" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="318" ht="12.800000000000001">
       <c r="A318" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="319" ht="12.800000000000001">
       <c r="A319" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row r="320" ht="12.800000000000001">
       <c r="A320" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="321" ht="12.800000000000001">
       <c r="A321" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="322" ht="12.800000000000001">
@@ -5142,7 +5142,7 @@
     </row>
     <row r="324" ht="12.800000000000001">
       <c r="A324" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
     </row>
     <row r="325" ht="12.800000000000001">
@@ -5192,7 +5192,7 @@
     </row>
     <row r="334" ht="12.800000000000001">
       <c r="A334" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="335" ht="12.800000000000001">
@@ -5217,7 +5217,7 @@
     </row>
     <row r="339" ht="12.800000000000001">
       <c r="A339" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="340" ht="12.800000000000001">
@@ -5227,7 +5227,7 @@
     </row>
     <row r="341" ht="12.800000000000001">
       <c r="A341" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="342" ht="12.800000000000001">
@@ -5262,7 +5262,7 @@
     </row>
     <row r="348" ht="12.800000000000001">
       <c r="A348" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="349" ht="12.800000000000001">
@@ -5292,7 +5292,7 @@
     </row>
     <row r="354" ht="12.800000000000001">
       <c r="A354" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="355" ht="12.800000000000001">
@@ -5307,7 +5307,7 @@
     </row>
     <row r="357" ht="12.800000000000001">
       <c r="A357" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="358" ht="12.800000000000001">
@@ -5367,7 +5367,7 @@
     </row>
     <row r="369" ht="12.800000000000001">
       <c r="A369" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="370" ht="12.800000000000001">
@@ -5377,7 +5377,7 @@
     </row>
     <row r="371" ht="12.800000000000001">
       <c r="A371" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="372" ht="12.800000000000001">
@@ -5432,12 +5432,12 @@
     </row>
     <row r="382" ht="12.800000000000001">
       <c r="A382" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="383" ht="12.800000000000001">
       <c r="A383" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="384" ht="12.800000000000001">
@@ -5452,12 +5452,12 @@
     </row>
     <row r="386" ht="12.800000000000001">
       <c r="A386" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="387" ht="12.800000000000001">
       <c r="A387" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
     </row>
     <row r="388" ht="12.800000000000001">

</xml_diff>